<commit_message>
-Adjusted the one test dichotomous and finished polytomous test.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_polytomous_analysis.xlsx
+++ b/Data analytics/Language tests/Data/one_test_polytomous_analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>Student</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>% Correct</t>
-  </si>
-  <si>
     <t>z</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
   </si>
   <si>
     <t>Student30</t>
-  </si>
-  <si>
-    <t>MAX POSS.</t>
   </si>
   <si>
     <t>Item facility</t>
@@ -358,7 +352,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="distribution_of_scores.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="distribution_of_polytomous_scores.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -385,9 +379,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Y33" totalsRowShown="0">
-  <autoFilter ref="A1:Y33"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X31" totalsRowShown="0">
+  <autoFilter ref="A1:X31"/>
+  <tableColumns count="24">
     <tableColumn id="1" name="Student"/>
     <tableColumn id="2" name="Q01"/>
     <tableColumn id="3" name="Q02"/>
@@ -410,9 +404,8 @@
     <tableColumn id="20" name="Q19"/>
     <tableColumn id="21" name="Q20"/>
     <tableColumn id="22" name="Total"/>
-    <tableColumn id="23" name="% Correct"/>
-    <tableColumn id="24" name="z"/>
-    <tableColumn id="25" name="T"/>
+    <tableColumn id="23" name="z"/>
+    <tableColumn id="24" name="T"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -703,13 +696,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:X69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,13 +775,10 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>25</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -854,18 +844,15 @@
         <v>14.5</v>
       </c>
       <c r="W2">
-        <v>72.5</v>
+        <v>-1.1</v>
       </c>
       <c r="X2">
-        <v>-0.8</v>
-      </c>
-      <c r="Y2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -931,18 +918,15 @@
         <v>30</v>
       </c>
       <c r="W3">
-        <v>150</v>
+        <v>1.3</v>
       </c>
       <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1008,18 +992,15 @@
         <v>16.5</v>
       </c>
       <c r="W4">
-        <v>82.5</v>
+        <v>-0.7</v>
       </c>
       <c r="X4">
-        <v>-0.6</v>
-      </c>
-      <c r="Y4">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1085,18 +1066,15 @@
         <v>14.5</v>
       </c>
       <c r="W5">
-        <v>72.5</v>
+        <v>-1.1</v>
       </c>
       <c r="X5">
-        <v>-0.8</v>
-      </c>
-      <c r="Y5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1162,18 +1140,15 @@
         <v>27.5</v>
       </c>
       <c r="W6">
-        <v>137.5</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.7</v>
-      </c>
-      <c r="Y6">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1239,18 +1214,15 @@
         <v>29</v>
       </c>
       <c r="W7">
-        <v>145</v>
+        <v>1.2</v>
       </c>
       <c r="X7">
-        <v>0.9</v>
-      </c>
-      <c r="Y7">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1316,18 +1288,15 @@
         <v>18.5</v>
       </c>
       <c r="W8">
-        <v>92.5</v>
+        <v>-0.4</v>
       </c>
       <c r="X8">
-        <v>-0.3</v>
-      </c>
-      <c r="Y8">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1393,18 +1362,15 @@
         <v>21</v>
       </c>
       <c r="W9">
-        <v>105</v>
+        <v>-0.1</v>
       </c>
       <c r="X9">
-        <v>-0</v>
-      </c>
-      <c r="Y9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1470,18 +1436,15 @@
         <v>36</v>
       </c>
       <c r="W10">
-        <v>180</v>
+        <v>2.3</v>
       </c>
       <c r="X10">
-        <v>1.7</v>
-      </c>
-      <c r="Y10">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1547,18 +1510,15 @@
         <v>28</v>
       </c>
       <c r="W11">
-        <v>140</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>0.8</v>
-      </c>
-      <c r="Y11">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1624,18 +1584,15 @@
         <v>15.5</v>
       </c>
       <c r="W12">
-        <v>77.5</v>
+        <v>-0.9</v>
       </c>
       <c r="X12">
-        <v>-0.7</v>
-      </c>
-      <c r="Y12">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1701,18 +1658,15 @@
         <v>15.5</v>
       </c>
       <c r="W13">
-        <v>77.5</v>
+        <v>-0.9</v>
       </c>
       <c r="X13">
-        <v>-0.7</v>
-      </c>
-      <c r="Y13">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1778,18 +1732,15 @@
         <v>20.5</v>
       </c>
       <c r="W14">
-        <v>102.5</v>
+        <v>-0.1</v>
       </c>
       <c r="X14">
-        <v>-0.1</v>
-      </c>
-      <c r="Y14">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1855,18 +1806,15 @@
         <v>25</v>
       </c>
       <c r="W15">
-        <v>125</v>
+        <v>0.6</v>
       </c>
       <c r="X15">
-        <v>0.4</v>
-      </c>
-      <c r="Y15">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1932,18 +1880,15 @@
         <v>18.5</v>
       </c>
       <c r="W16">
-        <v>92.5</v>
+        <v>-0.4</v>
       </c>
       <c r="X16">
-        <v>-0.3</v>
-      </c>
-      <c r="Y16">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2009,18 +1954,15 @@
         <v>22</v>
       </c>
       <c r="W17">
-        <v>110</v>
+        <v>0.1</v>
       </c>
       <c r="X17">
-        <v>0.1</v>
-      </c>
-      <c r="Y17">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2086,18 +2028,15 @@
         <v>22</v>
       </c>
       <c r="W18">
-        <v>110</v>
+        <v>0.1</v>
       </c>
       <c r="X18">
-        <v>0.1</v>
-      </c>
-      <c r="Y18">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2163,18 +2102,15 @@
         <v>24.5</v>
       </c>
       <c r="W19">
-        <v>122.5</v>
+        <v>0.5</v>
       </c>
       <c r="X19">
-        <v>0.4</v>
-      </c>
-      <c r="Y19">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2240,18 +2176,15 @@
         <v>22.5</v>
       </c>
       <c r="W20">
-        <v>112.5</v>
+        <v>0.2</v>
       </c>
       <c r="X20">
-        <v>0.1</v>
-      </c>
-      <c r="Y20">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2317,18 +2250,15 @@
         <v>18.5</v>
       </c>
       <c r="W21">
-        <v>92.5</v>
+        <v>-0.4</v>
       </c>
       <c r="X21">
-        <v>-0.3</v>
-      </c>
-      <c r="Y21">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2394,18 +2324,15 @@
         <v>19</v>
       </c>
       <c r="W22">
-        <v>95</v>
+        <v>-0.4</v>
       </c>
       <c r="X22">
-        <v>-0.3</v>
-      </c>
-      <c r="Y22">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2471,18 +2398,15 @@
         <v>14</v>
       </c>
       <c r="W23">
-        <v>70</v>
+        <v>-1.1</v>
       </c>
       <c r="X23">
-        <v>-0.9</v>
-      </c>
-      <c r="Y23">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2548,18 +2472,15 @@
         <v>23</v>
       </c>
       <c r="W24">
-        <v>115</v>
+        <v>0.3</v>
       </c>
       <c r="X24">
-        <v>0.2</v>
-      </c>
-      <c r="Y24">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2625,18 +2546,15 @@
         <v>32</v>
       </c>
       <c r="W25">
-        <v>160</v>
+        <v>1.7</v>
       </c>
       <c r="X25">
-        <v>1.3</v>
-      </c>
-      <c r="Y25">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2702,18 +2620,15 @@
         <v>6.5</v>
       </c>
       <c r="W26">
-        <v>32.5</v>
+        <v>-2.3</v>
       </c>
       <c r="X26">
-        <v>-1.8</v>
-      </c>
-      <c r="Y26">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2779,18 +2694,15 @@
         <v>23</v>
       </c>
       <c r="W27">
-        <v>115</v>
+        <v>0.3</v>
       </c>
       <c r="X27">
-        <v>0.2</v>
-      </c>
-      <c r="Y27">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2856,18 +2768,15 @@
         <v>10</v>
       </c>
       <c r="W28">
-        <v>50</v>
+        <v>-1.8</v>
       </c>
       <c r="X28">
-        <v>-1.4</v>
-      </c>
-      <c r="Y28">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2933,18 +2842,15 @@
         <v>25</v>
       </c>
       <c r="W29">
-        <v>125</v>
+        <v>0.6</v>
       </c>
       <c r="X29">
-        <v>0.4</v>
-      </c>
-      <c r="Y29">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3010,18 +2916,15 @@
         <v>20</v>
       </c>
       <c r="W30">
-        <v>100</v>
+        <v>-0.2</v>
       </c>
       <c r="X30">
-        <v>-0.2</v>
-      </c>
-      <c r="Y30">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:24">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3087,876 +2990,752 @@
         <v>27.5</v>
       </c>
       <c r="W31">
-        <v>137.5</v>
+        <v>1</v>
       </c>
       <c r="X31">
-        <v>0.7</v>
-      </c>
-      <c r="Y31">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <v>0</v>
-      </c>
-      <c r="X32">
-        <v>-2.5</v>
-      </c>
-      <c r="Y32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25">
-      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>4</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="J33">
-        <v>3</v>
-      </c>
-      <c r="K33">
-        <v>2</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33">
-        <v>3</v>
-      </c>
-      <c r="N33">
-        <v>2</v>
-      </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="P33">
-        <v>2</v>
-      </c>
-      <c r="Q33">
-        <v>3</v>
-      </c>
-      <c r="R33">
-        <v>4</v>
-      </c>
-      <c r="S33">
-        <v>1</v>
-      </c>
-      <c r="T33">
-        <v>2</v>
-      </c>
-      <c r="U33">
-        <v>3</v>
-      </c>
-      <c r="V33">
-        <v>45</v>
-      </c>
-      <c r="W33">
-        <v>225</v>
-      </c>
-      <c r="X33">
-        <v>2.8</v>
-      </c>
-      <c r="Y33">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25">
+      <c r="B35">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="C35">
+        <v>0.4</v>
+      </c>
+      <c r="D35">
+        <v>0.3777777777777778</v>
+      </c>
+      <c r="E35">
+        <v>0.4833333333333333</v>
+      </c>
+      <c r="F35">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="G35">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="H35">
+        <v>0.4333333333333333</v>
+      </c>
+      <c r="I35">
+        <v>0.3666666666666666</v>
+      </c>
+      <c r="J35">
+        <v>0.4555555555555555</v>
+      </c>
+      <c r="K35">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="L35">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="M35">
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="N35">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="O35">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="P35">
+        <v>0.45</v>
+      </c>
+      <c r="Q35">
+        <v>0.3</v>
+      </c>
+      <c r="R35">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="S35">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="T35">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="U35">
+        <v>0.4666666666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25">
+      <c r="B36">
+        <v>0.7</v>
+      </c>
+      <c r="C36">
+        <v>0.6</v>
+      </c>
+      <c r="D36">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="E36">
+        <v>0.6</v>
+      </c>
+      <c r="F36">
+        <v>0.75</v>
+      </c>
+      <c r="G36">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="H36">
+        <v>0.6</v>
+      </c>
+      <c r="I36">
+        <v>0.6</v>
+      </c>
+      <c r="J36">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="K36">
+        <v>0.45</v>
+      </c>
+      <c r="L36">
+        <v>0.55</v>
+      </c>
+      <c r="M36">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="N36">
+        <v>0.55</v>
+      </c>
+      <c r="O36">
+        <v>0.6</v>
+      </c>
+      <c r="P36">
+        <v>0.6</v>
+      </c>
+      <c r="Q36">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="R36">
+        <v>0.775</v>
+      </c>
+      <c r="S36">
+        <v>0.6</v>
+      </c>
+      <c r="T36">
+        <v>0.65</v>
+      </c>
+      <c r="U36">
+        <v>0.4666666666666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B37">
-        <v>0.548</v>
+        <v>0.3</v>
       </c>
       <c r="C37">
-        <v>0.839</v>
+        <v>0.15</v>
       </c>
       <c r="D37">
-        <v>1.194</v>
+        <v>0.2</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F37">
-        <v>2.129</v>
+        <v>0.25</v>
       </c>
       <c r="G37">
-        <v>1.645</v>
+        <v>0.4</v>
       </c>
       <c r="H37">
-        <v>0.452</v>
+        <v>0.2</v>
       </c>
       <c r="I37">
-        <v>0.774</v>
+        <v>0.4</v>
       </c>
       <c r="J37">
-        <v>1.419</v>
+        <v>0.2</v>
       </c>
       <c r="K37">
-        <v>0.968</v>
+        <v>0.55</v>
       </c>
       <c r="L37">
-        <v>0.548</v>
+        <v>0.5</v>
       </c>
       <c r="M37">
-        <v>1.677</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="N37">
-        <v>0.968</v>
+        <v>0.3</v>
       </c>
       <c r="O37">
-        <v>0.355</v>
+        <v>0.1</v>
       </c>
       <c r="P37">
-        <v>0.9350000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="Q37">
-        <v>0.968</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="R37">
-        <v>2.387</v>
+        <v>0.3</v>
       </c>
       <c r="S37">
-        <v>0.581</v>
+        <v>0.7</v>
       </c>
       <c r="T37">
-        <v>1.258</v>
+        <v>0.55</v>
       </c>
       <c r="U37">
-        <v>1.452</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25">
-      <c r="A38" s="1" t="s">
+        <v>0.5333333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B38">
-        <v>0.8</v>
-      </c>
-      <c r="C38">
-        <v>1.2</v>
-      </c>
-      <c r="D38">
-        <v>2.2</v>
-      </c>
-      <c r="E38">
-        <v>1.4</v>
-      </c>
-      <c r="F38">
-        <v>3.3</v>
-      </c>
-      <c r="G38">
-        <v>2.2</v>
-      </c>
-      <c r="H38">
-        <v>0.6</v>
-      </c>
-      <c r="I38">
-        <v>1.2</v>
-      </c>
-      <c r="J38">
-        <v>2.2</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38">
-        <v>0.6</v>
-      </c>
-      <c r="M38">
-        <v>2.1</v>
-      </c>
-      <c r="N38">
-        <v>1.3</v>
-      </c>
-      <c r="O38">
-        <v>0.7</v>
-      </c>
-      <c r="P38">
-        <v>1.3</v>
-      </c>
-      <c r="Q38">
-        <v>1.8</v>
-      </c>
-      <c r="R38">
-        <v>3.1</v>
-      </c>
-      <c r="S38">
-        <v>0.7</v>
-      </c>
-      <c r="T38">
-        <v>1.4</v>
-      </c>
-      <c r="U38">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B39">
-        <v>0.111</v>
-      </c>
-      <c r="C39">
-        <v>0.333</v>
-      </c>
-      <c r="D39">
-        <v>0.667</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0.889</v>
-      </c>
-      <c r="G39">
-        <v>1.444</v>
-      </c>
-      <c r="H39">
-        <v>0.111</v>
-      </c>
-      <c r="I39">
-        <v>0.667</v>
-      </c>
-      <c r="J39">
-        <v>0.333</v>
-      </c>
-      <c r="K39">
-        <v>1.333</v>
-      </c>
-      <c r="L39">
+      <c r="B40">
+        <v>0.4</v>
+      </c>
+      <c r="C40">
+        <v>0.45</v>
+      </c>
+      <c r="D40">
+        <v>0.4333333333333333</v>
+      </c>
+      <c r="E40">
         <v>0.5</v>
       </c>
-      <c r="M39">
-        <v>1.222</v>
-      </c>
-      <c r="N39">
-        <v>0.556</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0.444</v>
-      </c>
-      <c r="Q39">
-        <v>0.667</v>
-      </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-      <c r="S39">
-        <v>0.778</v>
-      </c>
-      <c r="T39">
-        <v>1</v>
-      </c>
-      <c r="U39">
-        <v>1.889</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25">
+      <c r="F40">
+        <v>0.5</v>
+      </c>
+      <c r="G40">
+        <v>0.3333333333333334</v>
+      </c>
+      <c r="H40">
+        <v>0.4</v>
+      </c>
+      <c r="I40">
+        <v>0.2</v>
+      </c>
+      <c r="J40">
+        <v>0.5333333333333334</v>
+      </c>
+      <c r="K40">
+        <v>-0.1</v>
+      </c>
+      <c r="L40">
+        <v>0.05000000000000004</v>
+      </c>
+      <c r="M40">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="N40">
+        <v>0.2500000000000001</v>
+      </c>
+      <c r="O40">
+        <v>0.5</v>
+      </c>
+      <c r="P40">
+        <v>0.35</v>
+      </c>
+      <c r="Q40">
+        <v>0.4</v>
+      </c>
+      <c r="R40">
+        <v>0.475</v>
+      </c>
+      <c r="S40">
+        <v>-0.09999999999999998</v>
+      </c>
+      <c r="T40">
+        <v>0.09999999999999998</v>
+      </c>
+      <c r="U40">
+        <v>-0.06666666666666671</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="B41">
+        <v>0.52</v>
+      </c>
+      <c r="C41">
+        <v>0.438</v>
+      </c>
+      <c r="D41">
+        <v>0.517</v>
+      </c>
+      <c r="E41">
+        <v>0.534</v>
+      </c>
+      <c r="F41">
+        <v>0.709</v>
+      </c>
+      <c r="G41">
+        <v>0.339</v>
+      </c>
+      <c r="H41">
+        <v>0.341</v>
+      </c>
+      <c r="I41">
+        <v>0.293</v>
+      </c>
+      <c r="J41">
+        <v>0.586</v>
+      </c>
+      <c r="K41">
+        <v>-0.126</v>
+      </c>
+      <c r="L41">
+        <v>0.045</v>
+      </c>
+      <c r="M41">
+        <v>0.215</v>
+      </c>
+      <c r="N41">
+        <v>0.421</v>
+      </c>
+      <c r="O41">
+        <v>0.556</v>
+      </c>
+      <c r="P41">
+        <v>0.507</v>
+      </c>
+      <c r="Q41">
+        <v>0.529</v>
+      </c>
+      <c r="R41">
+        <v>0.615</v>
+      </c>
+      <c r="S41">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="T41">
+        <v>0.147</v>
+      </c>
+      <c r="U41">
+        <v>-0.114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1">
         <v>4</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G43" s="1">
         <v>5</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H43" s="1">
         <v>6</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I43" s="1">
         <v>7</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J43" s="1">
         <v>8</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K43" s="1">
         <v>9</v>
       </c>
-      <c r="K41" s="1" t="s">
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
         <v>10</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="E45" t="s">
         <v>11</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="F45" t="s">
         <v>12</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="G45" t="s">
         <v>13</v>
       </c>
-      <c r="O41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P41" s="1" t="s">
+      <c r="H45" t="s">
         <v>15</v>
       </c>
-      <c r="Q41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S41" s="1" t="s">
+      <c r="I45" t="s">
         <v>18</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="J45" t="s">
         <v>19</v>
       </c>
-      <c r="U41" s="1" t="s">
+      <c r="K45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
-      <c r="A42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42">
-        <v>0.6890000000000001</v>
-      </c>
-      <c r="C42">
-        <v>0.867</v>
-      </c>
-      <c r="D42">
-        <v>1.533</v>
-      </c>
-      <c r="E42">
-        <v>1.4</v>
-      </c>
-      <c r="F42">
-        <v>2.411</v>
-      </c>
-      <c r="G42">
-        <v>0.7560000000000002</v>
-      </c>
-      <c r="H42">
-        <v>0.489</v>
-      </c>
-      <c r="I42">
-        <v>0.5329999999999999</v>
-      </c>
-      <c r="J42">
-        <v>1.867</v>
-      </c>
-      <c r="K42">
-        <v>-0.333</v>
-      </c>
-      <c r="L42">
-        <v>0.09999999999999998</v>
-      </c>
-      <c r="M42">
-        <v>0.8780000000000001</v>
-      </c>
-      <c r="N42">
-        <v>0.744</v>
-      </c>
-      <c r="O42">
-        <v>0.7</v>
-      </c>
-      <c r="P42">
-        <v>0.8560000000000001</v>
-      </c>
-      <c r="Q42">
-        <v>1.133</v>
-      </c>
-      <c r="R42">
-        <v>2.1</v>
-      </c>
-      <c r="S42">
-        <v>-0.07800000000000007</v>
-      </c>
-      <c r="T42">
-        <v>0.3999999999999999</v>
-      </c>
-      <c r="U42">
-        <v>-0.4890000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25">
-      <c r="A43" s="1" t="s">
+    <row r="46" spans="1:21">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B43">
-        <v>0.519</v>
-      </c>
-      <c r="C43">
-        <v>0.492</v>
-      </c>
-      <c r="D43">
-        <v>0.571</v>
-      </c>
-      <c r="E43">
-        <v>0.554</v>
-      </c>
-      <c r="F43">
-        <v>0.717</v>
-      </c>
-      <c r="G43">
-        <v>0.397</v>
-      </c>
-      <c r="H43">
-        <v>0.389</v>
-      </c>
-      <c r="I43">
-        <v>0.369</v>
-      </c>
-      <c r="J43">
-        <v>0.602</v>
-      </c>
-      <c r="K43">
-        <v>0.024</v>
-      </c>
-      <c r="L43">
-        <v>0.16</v>
-      </c>
-      <c r="M43">
-        <v>0.303</v>
-      </c>
-      <c r="N43">
-        <v>0.48</v>
-      </c>
-      <c r="O43">
-        <v>0.585</v>
-      </c>
-      <c r="P43">
-        <v>0.545</v>
-      </c>
-      <c r="Q43">
-        <v>0.614</v>
-      </c>
-      <c r="R43">
-        <v>0.622</v>
-      </c>
-      <c r="S43">
-        <v>0.028</v>
-      </c>
-      <c r="T43">
-        <v>0.219</v>
-      </c>
-      <c r="U43">
-        <v>0.033</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25">
-      <c r="A45" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="1">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>2</v>
-      </c>
-      <c r="E45" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25">
-      <c r="A46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25">
-      <c r="A47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25">
-      <c r="A48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="B50">
+        <v>21.333</v>
+      </c>
+      <c r="C50">
+        <v>0.01</v>
+      </c>
+      <c r="D50">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="B51">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B52">
-        <v>21.406</v>
-      </c>
-      <c r="C52">
-        <v>107.031</v>
-      </c>
-      <c r="D52">
-        <v>0.003</v>
-      </c>
-      <c r="E52">
-        <v>50.031</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B53">
-        <v>18.5</v>
-      </c>
-      <c r="C53">
-        <v>92.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B54">
-        <v>16.25</v>
-      </c>
-      <c r="C54">
-        <v>81.25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B55">
-        <v>21.5</v>
-      </c>
-      <c r="C55">
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B56">
-        <v>25.625</v>
-      </c>
-      <c r="C56">
-        <v>128.125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B57">
-        <v>45</v>
-      </c>
-      <c r="C57">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>6.448</v>
       </c>
       <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>1.008</v>
+      </c>
+      <c r="D58">
+        <v>10.081</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B59">
-        <v>46</v>
-      </c>
-      <c r="C59">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>6.558</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B60">
-        <v>8.407999999999999</v>
-      </c>
-      <c r="C60">
-        <v>42.04</v>
-      </c>
-      <c r="D60">
-        <v>0.996</v>
-      </c>
-      <c r="E60">
-        <v>9.958</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>41.572</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B61">
-        <v>8.542999999999999</v>
-      </c>
-      <c r="C61">
-        <v>42.713</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>43.006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B62">
-        <v>70.694</v>
-      </c>
-      <c r="C62">
-        <v>17.674</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B63">
-        <v>72.97499999999999</v>
-      </c>
-      <c r="C63">
-        <v>18.244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B64">
-        <v>4.688</v>
-      </c>
-      <c r="C64">
-        <v>23.438</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B65">
-        <v>32</v>
-      </c>
-      <c r="C65">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>0.427</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B66">
-        <v>0.17</v>
-      </c>
-      <c r="C66">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B67">
-        <v>0.414</v>
-      </c>
-      <c r="C67">
-        <v>0.414</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>0.078</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B68">
-        <v>0.411</v>
-      </c>
-      <c r="C68">
-        <v>0.411</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>0.833</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B69">
-        <v>1.604</v>
-      </c>
-      <c r="C69">
-        <v>1.604</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70">
-        <v>0.8090000000000001</v>
-      </c>
-      <c r="C70">
-        <v>0.8090000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71">
-        <v>1.981</v>
-      </c>
-      <c r="C71">
-        <v>1.981</v>
+        <v>0.094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>